<commit_message>
LTC6811 and SPICE Sim
</commit_message>
<xml_diff>
--- a/Boards/Tractive System/IFE_BMSSlave_2019/LTC6811/BOM.xlsx
+++ b/Boards/Tractive System/IFE_BMSSlave_2019/LTC6811/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chait\Documents\WSL\IFE_2019_Hardware\Boards\Tractive System\IFE_BMSSlave_2019\LTC6811\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB28E716-917A-4A14-A169-6730FC36F0D3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E13FE8-375E-4826-8463-BB512A304D04}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF0F842-A7B8-4128-83CE-90309877C382}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>PN</t>
   </si>
@@ -48,15 +48,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>BUK78150-55A/CUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Nexperia/BUK78150-55A-CUX?qs=sGAEpiMZZMshyDBzk1%2FWi5%252B%2F6t%2FTU9Z71z3ZevR7qF%252BAx%2FgFH%2FrXSA%3D%3D </t>
-  </si>
-  <si>
-    <t>NX7002AKVL</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.mouser.com/ProductDetail/Nexperia/NX7002AKVL?qs=sGAEpiMZZMshyDBzk1%2FWiwhg%252BJbteykV9w5cubKq8XdkO9kd8b8Ncw%3D%3D </t>
   </si>
   <si>
@@ -75,25 +66,79 @@
     <t xml:space="preserve">https://www.mouser.com/ProductDetail/KEMET/T491A105K035AT?qs=sGAEpiMZZMtZ1n0r9vR22SjDo%2FRaJSx%252BBJL0n6HcLrI%3D </t>
   </si>
   <si>
-    <t>SOT223 NMOS</t>
-  </si>
-  <si>
-    <t>SOT23 NMOS</t>
-  </si>
-  <si>
-    <t>2512 Resistor</t>
-  </si>
-  <si>
-    <t>35205R1JT</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/TE-Connectivity-CGS/35205R1JT?qs=sGAEpiMZZMtlubZbdhIBIIenWIH7rhEvbgBWa%252B1LO6w%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Texas-Instruments/LP2951-50DR?qs=sGAEpiMZZMsGz1a6aV8DcKyc140gPNQr88A2RaMW6L0%3D</t>
   </si>
   <si>
     <t>LP2951-50DR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/ON-Semiconductor/1SMB5928BT3G?qs=sGAEpiMZZMtQ8nqTKtFS%2FJ7m6e1KBCguI5yOdiThkFg%3D </t>
+  </si>
+  <si>
+    <t>13V zener</t>
+  </si>
+  <si>
+    <t>1SMB5928BT3G</t>
+  </si>
+  <si>
+    <t>DPAK NMOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Vishay-Siliconix/IRLR110TRPBF?qs=sGAEpiMZZMshyDBzk1%2FWi4bBo6KWdDd5qUueznBjLB8%3D </t>
+  </si>
+  <si>
+    <t>IRLR110TRPBF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Murata-Electronics/PRF15BC102RB6RC?qs=sGAEpiMZZMsAYIPNLIqEPNIz%252BwQ02jVW8WQh6KSc6Bc%3D</t>
+  </si>
+  <si>
+    <t>PTC thermistor</t>
+  </si>
+  <si>
+    <t>PRF15BC102RB6RC</t>
+  </si>
+  <si>
+    <t>Right angle crimps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Molex/35021-1201-Cut-Strip?qs=sGAEpiMZZMs%252BGHln7q6pm%252Bv5BXf4QdrTy6nfkib2RIB4OwsSNmw8Ew%3D%3D </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.com/ProductDetail/Molex/35023-0002?qs=%2Fha2pyFaduiIAmZSevuPTdYQqsJYR9ufMysb9X1F8SY%3D </t>
+  </si>
+  <si>
+    <t>35021-1201</t>
+  </si>
+  <si>
+    <t>35023-0002</t>
+  </si>
+  <si>
+    <t>Right angle housings</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>SOT23 PMOS</t>
+  </si>
+  <si>
+    <t>BSS84-7-F</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Bel-Fuse/C1F-25?qs=sGAEpiMZZMtxU2g%2F1juGqTi%252BNtKN7qu4Nt8x0xmmQvtWYBQVO0WEHA%3D%3D</t>
+  </si>
+  <si>
+    <t>C1F 2.5</t>
+  </si>
+  <si>
+    <t>2.5A Fuse</t>
   </si>
 </sst>
 </file>
@@ -456,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{013C58FE-AC27-4F75-9C9B-266AB5A1DA65}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +515,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -490,83 +535,80 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C2">
-        <v>0.17599999999999999</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>17.599999999999998</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C3">
-        <v>0.04</v>
+        <v>0.65</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E13" si="0">C3*D3</f>
-        <v>4</v>
+        <f>C3*D3</f>
+        <v>10.4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="D4">
-        <v>1000</v>
+        <v>16</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>66</v>
+        <f t="shared" ref="E4:E14" si="0">C4*D4</f>
+        <v>1.056</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5">
-        <v>0.48</v>
+        <v>0.187</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>7.1999999999999993</v>
+        <v>2.992</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>19</v>
@@ -574,53 +616,128 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6">
+        <v>0.48</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
         <v>0.23499999999999999</v>
       </c>
-      <c r="D6">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>3.5249999999999999</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="C8">
+        <v>0.316</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>0.03</v>
+      </c>
+      <c r="D9">
+        <v>32</v>
+      </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.96</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>0.184</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.944</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -635,18 +752,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17">
-        <f>SUM(E2:E13)</f>
-        <v>98.325000000000003</v>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <f>SUM(E2:E14)</f>
+        <v>31.150000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19">
+        <f>E18*7</f>
+        <v>218.05</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{81FF9E92-FE7A-4622-9708-909FB6B538B6}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{2EC47ABA-0623-4969-AC62-4067FB33812A}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{8C8B4CE7-3058-4F65-A89F-3812C9C12493}"/>
-    <hyperlink ref="F4" r:id="rId4" xr:uid="{38833A39-DA96-4E96-B37E-2EB2026BFA42}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{2EC47ABA-0623-4969-AC62-4067FB33812A}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{8C8B4CE7-3058-4F65-A89F-3812C9C12493}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{E8C17BA0-3E53-4C22-84AC-77763FB6B564}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{61C93175-3317-40FF-8E27-1A4A9BBD7B8C}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{1143D09D-8107-4E28-85C9-D71EF107B085}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{31C1CFEA-2461-4097-96D0-A4EECD7710BF}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{E7183BED-1DED-4DA0-8902-E1B7BD0634C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>